<commit_message>
Done produce Figure 1. Waiting for comparison
</commit_message>
<xml_diff>
--- a/PortfolioVIX.xlsx
+++ b/PortfolioVIX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seacen-my.sharepoint.com/personal/yassier_seacen_org/Documents/Desktop/Victor/GAR_Chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_C0F9B35B4436054091B663A5C44959442D344E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D77CD06A-5741-4AFA-AF0A-083CD00DC5DF}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_C0F9B35B4436054091B663A5C44959442D344E2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{904BEAE6-B66B-45E6-AA32-D378E3846FE8}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="300" windowWidth="20730" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,12 +79,23 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -107,7 +115,7 @@
       <tp t="e">
         <v>#N/A</v>
         <stp/>
-        <stp>{6B52AAE9-9160-4859-9B5A-E02C54665936}_x0000_</stp>
+        <stp>{BB1E9E99-E63F-49D0-B684-B67CFF3B3F82}_x0000_</stp>
         <tr r="A1" s="2"/>
       </tp>
     </main>
@@ -414,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C912"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A891" workbookViewId="0">
+      <selection activeCell="A891" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11364,6 +11372,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>